<commit_message>
[Pipette] F/W debugging, Manual 작성
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/3_Firmware/Plasma_Gen_debug manual.xlsx
+++ b/1_Plasma_Pipette/3_Firmware/Plasma_Gen_debug manual.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12FFCB9-FAAF-49D7-9780-7E98CDB71FA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tera Term 설정" sheetId="1" r:id="rId1"/>
     <sheet name="Debug command" sheetId="2" r:id="rId2"/>
+    <sheet name="FW Download" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Tera Term Set-up</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,14 +52,70 @@
   </si>
   <si>
     <t>동작중이 모든 function에 대한 debug massage가 올라옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. STM32 ST-LINK Utility 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Target &gt; Setting 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 아래와 같이 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Connect 버튼을 누르고, PCB의 reset S/W를 누르면 Connection이 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초기 Download가 안된 상태에서는 아래와 같이 모든 memory 영역이 F로 채워진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. Full chip erase 버튼을 선택하여 기존 Data를 지운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. Program verify 버튼을 선택하면 아래의 화면이 뜬다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Browse를 선택하여, Download하고자하는 Binary file를 선택하고, Start 버튼을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. Start 버튼을 선택하면, Download가 진행된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. Download가 완료되면, 아래와 같은 화면이 display 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Pipette F/W Download manual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◈ Pipette Download를 위한 H/W 구성도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette, JTAG PCB 구성도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST-Link/V2, JTAG PCB 구성도</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +129,32 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,8 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -129,7 +216,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -167,7 +260,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -205,7 +304,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -260,7 +365,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -303,7 +414,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -341,7 +458,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -362,6 +485,1031 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>46808</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>435428</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>8937</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{415E4B37-7BBB-42C5-9BA2-4BF99F5CFD17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="874122" y="525779"/>
+          <a:ext cx="6876506" cy="4926016"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>55644</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>69837</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9598484-F3E1-4ABE-8ED8-80346BCB75B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="903515" y="5933930"/>
+          <a:ext cx="6868885" cy="5021622"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>87086</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>195372</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>27761</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FEF8081-6C4E-4550-B4D2-FD21EAFE4FE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="11375571"/>
+          <a:ext cx="4571429" cy="6504762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>54430</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542104</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>174173</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E521CE4-40CF-4307-9C48-E2E9C11A376F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="881744" y="18581915"/>
+          <a:ext cx="6975560" cy="5105400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>43544</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>587830</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>215606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F8C4544-8E90-43A4-AC4D-CF79D692B1A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="870858" y="24242487"/>
+          <a:ext cx="7032172" cy="5146834"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>555172</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>32047</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>77343</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3E2958F-0DC6-4741-B181-3E70D0AA59BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1796143" y="25984200"/>
+          <a:ext cx="4876190" cy="1742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>97972</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>576944</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>167804</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33DC5C8A-AE2F-436C-A80A-75FF200C829C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="925286" y="29903058"/>
+          <a:ext cx="6966858" cy="5099031"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>337459</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>414334</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>210439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F23324B-20DB-4755-8EF9-DAFF57E2A09C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1578430" y="30610629"/>
+          <a:ext cx="5476190" cy="3780952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>97971</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>20451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3FB55B0-06FE-45B5-BD22-69DBE7914B6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="925285" y="40407772"/>
+          <a:ext cx="6988629" cy="5114965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>108858</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>500742</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>59974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="그림 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F9E2CE4-0E61-491D-A035-CE9C5880D7B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="936172" y="35585400"/>
+          <a:ext cx="6879770" cy="4316289"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>119744</xdr:colOff>
+      <xdr:row>211</xdr:row>
+      <xdr:rowOff>54430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>576943</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>130097</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDF346DA-CFF1-4940-81E4-FB567F685D30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="947058" y="45992144"/>
+          <a:ext cx="6945085" cy="5083095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>97971</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>225335</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>75110</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="그룹 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35CB0F67-18C6-463A-84B1-F00307B8878B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8599714" y="576942"/>
+          <a:ext cx="8901250" cy="4995454"/>
+          <a:chOff x="8763000" y="631371"/>
+          <a:chExt cx="8901249" cy="4995454"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="14" name="그림 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87C895F7-4B7D-44E9-876F-14DBB4291A3D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="8763000" y="631371"/>
+            <a:ext cx="8901249" cy="4995454"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="TextBox 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F169077A-D423-4B4C-9BA9-30544A211A7A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="14565086" y="3058886"/>
+            <a:ext cx="1192571" cy="447045"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>USB</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1600" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>충전기</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="TextBox 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B2D9D9-A37E-48C8-91E8-80F305890246}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16023771" y="4310743"/>
+            <a:ext cx="1105303" cy="342786"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ST-Link/V2</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="TextBox 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36AA6817-C27A-40EE-AF12-1877F2BDE7F7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11299372" y="3581400"/>
+            <a:ext cx="1241878" cy="342786"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Pipette USB</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>87086</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>343990</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>71847</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="23" name="그룹 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BF2C014-AEAA-4204-8812-2B04AEED9F7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8588829" y="6008915"/>
+          <a:ext cx="9030790" cy="3696789"/>
+          <a:chOff x="8469086" y="6531429"/>
+          <a:chExt cx="9030789" cy="3696789"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="15" name="그림 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9A84F66-A069-45D4-A0C2-E6D778322437}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="8469086" y="6531429"/>
+            <a:ext cx="9030789" cy="3696789"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="TextBox 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC0AB19-5D97-4E15-B7EE-CE4C6BEECF97}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="15087600" y="7805058"/>
+            <a:ext cx="1105303" cy="342786"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ST-Link/V2</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="TextBox 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{985DE39E-5574-4011-B19D-ED2CFF37B334}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10352315" y="7794171"/>
+            <a:ext cx="1192571" cy="447045"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>USB</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1600" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>충전기</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="TextBox 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4302529-7D1E-4CA5-AB6B-B83850782938}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8567057" y="8523514"/>
+            <a:ext cx="1241878" cy="342786"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Pipette USB</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -443,6 +1591,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -478,6 +1643,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -653,34 +1835,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="5" width="4.625" customWidth="1"/>
+    <col min="1" max="5" width="4.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C41" t="s">
         <v>3</v>
       </c>
@@ -693,20 +1875,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -714,7 +1896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -722,12 +1904,100 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52254C8C-8502-43DB-A69C-3B1D970C96E6}">
+  <dimension ref="A1:P211"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="5.3984375" customWidth="1"/>
+    <col min="2" max="2" width="3.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.3984375" customWidth="1"/>
+    <col min="14" max="14" width="4.19921875" customWidth="1"/>
+    <col min="15" max="15" width="4.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B52" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B84" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B111" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B137" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B163" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B185" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B211" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>